<commit_message>
added 2022 testes data
</commit_message>
<xml_diff>
--- a/Data/testes.xlsx
+++ b/Data/testes.xlsx
@@ -1,30 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11010"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jloveland\Dropbox\Max Planck notes\Ruffs Canada 2019\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martinbulla/Dropbox/Science/MS/ruff_sperm_v2/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB4C549C-6512-2048-9CB0-B98186459ED8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25125" windowHeight="14100"/>
+    <workbookView xWindow="14520" yWindow="460" windowWidth="25120" windowHeight="14100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="59">
   <si>
     <t>ID</t>
   </si>
@@ -186,12 +194,27 @@
   </si>
   <si>
     <t>Gonadmass</t>
+  </si>
+  <si>
+    <t>RdG/YLB</t>
+  </si>
+  <si>
+    <t>OdB/YdB</t>
+  </si>
+  <si>
+    <t>dGO/dGY</t>
+  </si>
+  <si>
+    <t>dGO/LBY</t>
+  </si>
+  <si>
+    <t>dGLB/YO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -228,7 +251,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -251,6 +274,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -530,24 +556,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:O41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="7" max="7" width="11.85546875" customWidth="1"/>
-    <col min="8" max="8" width="12.140625" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" customWidth="1"/>
-    <col min="11" max="11" width="10.7109375" customWidth="1"/>
-    <col min="14" max="14" width="11.5703125" customWidth="1"/>
+    <col min="7" max="7" width="11.83203125" customWidth="1"/>
+    <col min="8" max="8" width="12.1640625" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" customWidth="1"/>
+    <col min="11" max="11" width="10.6640625" customWidth="1"/>
+    <col min="14" max="14" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -594,7 +620,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="5">
         <v>1340</v>
       </c>
@@ -638,7 +664,7 @@
         <v>1.3718820861678005</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="5">
         <v>1311</v>
       </c>
@@ -678,11 +704,11 @@
         <v>3.75</v>
       </c>
       <c r="O3" s="10">
-        <f t="shared" ref="O3:O36" si="0">N3*100/K3</f>
+        <f t="shared" ref="O3:O41" si="0">N3*100/K3</f>
         <v>2.137970353477765</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
         <v>1312</v>
       </c>
@@ -726,7 +752,7 @@
         <v>1.7149615612063869</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
         <v>1330</v>
       </c>
@@ -774,7 +800,7 @@
         <v>1.3957123715944617</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="5">
         <v>1695</v>
       </c>
@@ -818,7 +844,7 @@
         <v>1.9631171921475312</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="5">
         <v>1306</v>
       </c>
@@ -866,7 +892,7 @@
         <v>1.2552799095722531</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="5">
         <v>1323</v>
       </c>
@@ -914,7 +940,7 @@
         <v>1.500771147229802</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="5">
         <v>1665</v>
       </c>
@@ -958,7 +984,7 @@
         <v>2.6602176541717051</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="5">
         <v>1672</v>
       </c>
@@ -1002,7 +1028,7 @@
         <v>1.7726737338044758</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="5">
         <v>1678</v>
       </c>
@@ -1046,7 +1072,7 @@
         <v>1.9320256818047945</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="5">
         <v>1685</v>
       </c>
@@ -1090,7 +1116,7 @@
         <v>1.6279069767441861</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="5">
         <v>1328</v>
       </c>
@@ -1138,7 +1164,7 @@
         <v>1.7634799337359055</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="5">
         <v>1674</v>
       </c>
@@ -1186,7 +1212,7 @@
         <v>1.8562874251497008</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="5">
         <v>372</v>
       </c>
@@ -1230,7 +1256,7 @@
         <v>1.7491926803013993</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="5">
         <v>370</v>
       </c>
@@ -1278,7 +1304,7 @@
         <v>2.2840172786177111</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="5">
         <v>319</v>
       </c>
@@ -1326,7 +1352,7 @@
         <v>1.2331304577930671</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" s="5">
         <v>1321</v>
       </c>
@@ -1370,7 +1396,7 @@
         <v>1.7520858164481525</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" s="5">
         <v>1324</v>
       </c>
@@ -1418,7 +1444,7 @@
         <v>1.984715410060454</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" s="5">
         <v>1645</v>
       </c>
@@ -1462,7 +1488,7 @@
         <v>1.9501822600243015</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" s="5">
         <v>1670</v>
       </c>
@@ -1510,7 +1536,7 @@
         <v>1.4077814077814079</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" s="5">
         <v>1680</v>
       </c>
@@ -1558,7 +1584,7 @@
         <v>2.1799047857679783</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" s="5">
         <v>1640</v>
       </c>
@@ -1606,7 +1632,7 @@
         <v>2.0465172769781992</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" s="5">
         <v>1693</v>
       </c>
@@ -1654,7 +1680,7 @@
         <v>1.7585890508716484</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" s="5">
         <v>374</v>
       </c>
@@ -1698,7 +1724,7 @@
         <v>1.7183908045977012</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" s="5">
         <v>1633</v>
       </c>
@@ -1746,7 +1772,7 @@
         <v>1.7481481481481482</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" s="5">
         <v>329</v>
       </c>
@@ -1794,7 +1820,7 @@
         <v>2.3955023221706186</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" s="5">
         <v>1015</v>
       </c>
@@ -1838,7 +1864,7 @@
         <v>1.7446043165467626</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" s="5">
         <v>1337</v>
       </c>
@@ -1886,7 +1912,7 @@
         <v>1.9130038715554545</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" s="5">
         <v>1319</v>
       </c>
@@ -1934,7 +1960,7 @@
         <v>2.6860865110151506</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" s="5">
         <v>1664</v>
       </c>
@@ -1978,7 +2004,7 @@
         <v>2.6502534395365678</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" s="5">
         <v>954</v>
       </c>
@@ -2026,7 +2052,7 @@
         <v>2.2248073287770826</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33" s="5">
         <v>1639</v>
       </c>
@@ -2074,7 +2100,7 @@
         <v>2.5304736923314302</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34" s="5">
         <v>1647</v>
       </c>
@@ -2122,7 +2148,7 @@
         <v>2.2249963283888969</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35" s="5">
         <v>1650</v>
       </c>
@@ -2170,7 +2196,7 @@
         <v>2.4461600975213327</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36" s="5">
         <v>672</v>
       </c>
@@ -2216,6 +2242,246 @@
       <c r="O36" s="10">
         <f t="shared" si="0"/>
         <v>2.7909070447895568</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>1378</v>
+      </c>
+      <c r="B37" t="s">
+        <v>7</v>
+      </c>
+      <c r="C37" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37" t="s">
+        <v>54</v>
+      </c>
+      <c r="E37">
+        <v>2019</v>
+      </c>
+      <c r="F37" s="14">
+        <v>3</v>
+      </c>
+      <c r="G37" s="15">
+        <v>44725</v>
+      </c>
+      <c r="H37">
+        <v>6</v>
+      </c>
+      <c r="I37">
+        <v>13</v>
+      </c>
+      <c r="J37">
+        <v>2022</v>
+      </c>
+      <c r="K37">
+        <v>131.5</v>
+      </c>
+      <c r="L37">
+        <v>1.6</v>
+      </c>
+      <c r="M37">
+        <v>1.7</v>
+      </c>
+      <c r="N37">
+        <v>3.3</v>
+      </c>
+      <c r="O37" s="16">
+        <f t="shared" si="0"/>
+        <v>2.5095057034220534</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>1357</v>
+      </c>
+      <c r="B38" t="s">
+        <v>7</v>
+      </c>
+      <c r="C38" t="s">
+        <v>4</v>
+      </c>
+      <c r="D38" t="s">
+        <v>55</v>
+      </c>
+      <c r="E38">
+        <v>2017</v>
+      </c>
+      <c r="F38" s="14">
+        <v>5</v>
+      </c>
+      <c r="G38" s="15">
+        <v>44725</v>
+      </c>
+      <c r="H38">
+        <v>6</v>
+      </c>
+      <c r="I38">
+        <v>13</v>
+      </c>
+      <c r="J38">
+        <v>2022</v>
+      </c>
+      <c r="K38">
+        <v>178</v>
+      </c>
+      <c r="L38">
+        <v>1.7</v>
+      </c>
+      <c r="M38">
+        <v>1.8</v>
+      </c>
+      <c r="N38">
+        <v>3.5</v>
+      </c>
+      <c r="O38" s="16">
+        <f t="shared" si="0"/>
+        <v>1.9662921348314606</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>1689</v>
+      </c>
+      <c r="B39" t="s">
+        <v>7</v>
+      </c>
+      <c r="C39" t="s">
+        <v>4</v>
+      </c>
+      <c r="D39" t="s">
+        <v>56</v>
+      </c>
+      <c r="E39">
+        <v>2010</v>
+      </c>
+      <c r="F39" s="14">
+        <v>12</v>
+      </c>
+      <c r="G39" s="15">
+        <v>44726</v>
+      </c>
+      <c r="H39">
+        <v>6</v>
+      </c>
+      <c r="I39">
+        <v>14</v>
+      </c>
+      <c r="J39">
+        <v>2022</v>
+      </c>
+      <c r="K39">
+        <v>169</v>
+      </c>
+      <c r="L39">
+        <v>1.2</v>
+      </c>
+      <c r="M39">
+        <v>1.2</v>
+      </c>
+      <c r="N39">
+        <v>2.4</v>
+      </c>
+      <c r="O39" s="16">
+        <f t="shared" si="0"/>
+        <v>1.4201183431952662</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>382</v>
+      </c>
+      <c r="B40" t="s">
+        <v>7</v>
+      </c>
+      <c r="C40" t="s">
+        <v>4</v>
+      </c>
+      <c r="D40" t="s">
+        <v>57</v>
+      </c>
+      <c r="E40">
+        <v>2010</v>
+      </c>
+      <c r="F40" s="14">
+        <v>12</v>
+      </c>
+      <c r="G40" s="15">
+        <v>44728</v>
+      </c>
+      <c r="H40">
+        <v>6</v>
+      </c>
+      <c r="I40">
+        <v>16</v>
+      </c>
+      <c r="J40">
+        <v>2022</v>
+      </c>
+      <c r="K40">
+        <v>186</v>
+      </c>
+      <c r="L40">
+        <v>1.8</v>
+      </c>
+      <c r="M40">
+        <v>2.1</v>
+      </c>
+      <c r="N40">
+        <v>3.9000000000000004</v>
+      </c>
+      <c r="O40" s="16">
+        <f t="shared" si="0"/>
+        <v>2.0967741935483875</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>1300</v>
+      </c>
+      <c r="B41" t="s">
+        <v>7</v>
+      </c>
+      <c r="C41" t="s">
+        <v>5</v>
+      </c>
+      <c r="D41" t="s">
+        <v>58</v>
+      </c>
+      <c r="E41">
+        <v>2014</v>
+      </c>
+      <c r="F41" s="14">
+        <v>8</v>
+      </c>
+      <c r="G41" s="15">
+        <v>44729</v>
+      </c>
+      <c r="H41">
+        <v>6</v>
+      </c>
+      <c r="I41">
+        <v>17</v>
+      </c>
+      <c r="J41">
+        <v>2022</v>
+      </c>
+      <c r="K41">
+        <v>182.4</v>
+      </c>
+      <c r="L41">
+        <v>1.8</v>
+      </c>
+      <c r="M41">
+        <v>1.6</v>
+      </c>
+      <c r="N41">
+        <v>3.4000000000000004</v>
+      </c>
+      <c r="O41" s="16">
+        <f t="shared" si="0"/>
+        <v>1.8640350877192986</v>
       </c>
     </row>
   </sheetData>

</xml_diff>